<commit_message>
fix: Change the position of MEMBERS in template.xlsx
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryuse/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryuse/Programming/typetalk_reminder/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D012A6-B09E-8843-ADDA-2CA9163299C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41155A9E-AFEC-A54B-AE19-AB14A4447471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -58,19 +58,7 @@
     <t>朝9時に送られるメッセージ</t>
   </si>
   <si>
-    <t>{MEMBERS}
-【リマインド】 本日{SCHEDULE_LEN}つの予定があります。
-{SCHEDULE}
-{ZOOM_TEXT}</t>
-  </si>
-  <si>
     <t>開始1時間前に送られるメッセージ</t>
-  </si>
-  <si>
-    <t>{MEMBERS}
-【リマインド】 もうすぐ以下の予定が開始されます。
-{SCHEDULE}
-{ZOOM_TEXT}</t>
   </si>
   <si>
     <t>接続先リンク(ZOOMのURLなど)</t>
@@ -118,6 +106,20 @@
   </si>
   <si>
     <t>サンプル３</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>【リマインド】 本日{SCHEDULE_LEN}つの予定があります。
+{SCHEDULE}
+{ZOOM_TEXT}
+{MEMBERS}</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>【リマインド】 もうすぐ以下の予定が開始されます。
+{SCHEDULE}
+{ZOOM_TEXT}
+{MEMBERS}</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -128,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="###0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -139,6 +141,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -146,6 +149,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -158,6 +162,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -193,6 +204,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -414,7 +428,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
@@ -477,7 +491,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -512,7 +526,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -572,17 +586,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -625,9 +639,9 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -640,47 +654,47 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>